<commit_message>
try catch read column
</commit_message>
<xml_diff>
--- a/NPOIHelperTest/TestImportExcel/test1.xlsx
+++ b/NPOIHelperTest/TestImportExcel/test1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5327C1C-51A8-48CB-975D-18A57126787D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A80725A-4EE9-4991-BB33-E61F13ECF9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,6 +95,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="177" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,7 +138,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -142,6 +146,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -484,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -494,7 +504,7 @@
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -514,7 +524,7 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -537,7 +547,7 @@
       <c r="E2">
         <v>1.69</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>32880.375752314816</v>
       </c>
       <c r="G2" s="1">
@@ -551,7 +561,12 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="F3" s="4">
+        <v>111</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -569,7 +584,7 @@
       <c r="E4">
         <v>1.69</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>32880</v>
       </c>
       <c r="G4" s="1">
@@ -592,7 +607,7 @@
       <c r="E5">
         <v>1.69</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>32881</v>
       </c>
       <c r="G5" s="1">
@@ -615,7 +630,7 @@
       <c r="E6">
         <v>1.69</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>32882</v>
       </c>
       <c r="G6" s="1">
@@ -638,7 +653,7 @@
       <c r="E7">
         <v>1.69</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>32883</v>
       </c>
       <c r="G7" s="1">
@@ -661,7 +676,7 @@
       <c r="E8">
         <v>1.69</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>32884</v>
       </c>
       <c r="G8" s="1">
@@ -684,7 +699,7 @@
       <c r="E9">
         <v>1.69</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>32885</v>
       </c>
       <c r="G9" s="1">
@@ -707,7 +722,7 @@
       <c r="E10">
         <v>1.69</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>32886</v>
       </c>
       <c r="G10" s="1">
@@ -730,7 +745,7 @@
       <c r="E11">
         <v>1.69</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>32887</v>
       </c>
       <c r="G11" s="1">
@@ -753,7 +768,7 @@
       <c r="E12">
         <v>1.69</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>32888</v>
       </c>
       <c r="G12" s="1">
@@ -776,7 +791,7 @@
       <c r="E13">
         <v>1.69</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>32889</v>
       </c>
       <c r="G13" s="1">
@@ -794,7 +809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>